<commit_message>
added step files for two-pcb stak up
</commit_message>
<xml_diff>
--- a/BOM/BOM-REV3.xlsx
+++ b/BOM/BOM-REV3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yann\Documents\GitHub\ATMEGA324_MTR_DRV_PCB\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6220A7B2-1C11-4FC2-A0F2-AC1951DDF9ED}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46F47BA4-7450-4954-BDBC-B5A2231E4EEF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="12375" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="984" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="246">
   <si>
     <t>Index</t>
   </si>
@@ -808,12 +808,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1130,8 +1133,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="M37" sqref="M37"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="D59" sqref="D59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1861,7 +1864,7 @@
       <c r="C23" t="s">
         <v>94</v>
       </c>
-      <c r="D23" s="2">
+      <c r="D23" s="5">
         <v>1935161</v>
       </c>
       <c r="E23" t="s">

</xml_diff>

<commit_message>
updated BOM for missing components
</commit_message>
<xml_diff>
--- a/BOM/BOM-REV3.xlsx
+++ b/BOM/BOM-REV3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yann\Documents\GitHub\ATMEGA324_MTR_DRV_PCB\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46F47BA4-7450-4954-BDBC-B5A2231E4EEF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24AF03C0-D378-4A07-96FE-7AC751BDDC12}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="12375" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="262">
   <si>
     <t>Index</t>
   </si>
@@ -665,9 +665,6 @@
     <t>DGTL ISO 2.5KV GEN PURP 8SOIC</t>
   </si>
   <si>
-    <t>U7-U8</t>
-  </si>
-  <si>
     <t>LM321MFX/NOPBCT-ND</t>
   </si>
   <si>
@@ -765,6 +762,57 @@
   </si>
   <si>
     <t>RES SMD 0 OHM JUMPER 1/16W 0402</t>
+  </si>
+  <si>
+    <t>C29</t>
+  </si>
+  <si>
+    <t>399-1169-1-ND</t>
+  </si>
+  <si>
+    <t>C0805C104M5RACTU</t>
+  </si>
+  <si>
+    <t>CAP CER 0.1UF 50V X7R 0805</t>
+  </si>
+  <si>
+    <t>RMCF0402FT120KCT-ND</t>
+  </si>
+  <si>
+    <t>RMCF0402FT120K</t>
+  </si>
+  <si>
+    <t>RES 120K OHM 1% 1/16W 0402</t>
+  </si>
+  <si>
+    <t>R27</t>
+  </si>
+  <si>
+    <t>SMA6J18AHR3GCT-ND</t>
+  </si>
+  <si>
+    <t>SMA6J18AHR3G</t>
+  </si>
+  <si>
+    <t>TVS DIODE 18V 28.3V DO214AC</t>
+  </si>
+  <si>
+    <t>D8</t>
+  </si>
+  <si>
+    <t>MBR0520LCT-ND</t>
+  </si>
+  <si>
+    <t>MBR0520L</t>
+  </si>
+  <si>
+    <t>DIODE SCHOTTKY 20V 500MA SOD123</t>
+  </si>
+  <si>
+    <t>D9</t>
+  </si>
+  <si>
+    <t>U7-U9</t>
   </si>
 </sst>
 </file>
@@ -1131,10 +1179,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J61"/>
+  <dimension ref="A1:J65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="D59" sqref="D59"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="F55" sqref="F55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1411,31 +1459,31 @@
         <v>8</v>
       </c>
       <c r="B9" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>38</v>
+        <v>246</v>
       </c>
       <c r="D9" t="s">
-        <v>39</v>
+        <v>247</v>
       </c>
       <c r="E9" t="s">
-        <v>40</v>
+        <v>248</v>
       </c>
       <c r="F9" t="s">
-        <v>41</v>
+        <v>245</v>
       </c>
       <c r="G9" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H9" s="2">
         <v>0</v>
       </c>
       <c r="I9">
-        <v>0.1</v>
+        <v>0.11</v>
       </c>
       <c r="J9" s="3">
-        <v>0.2</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -1443,22 +1491,22 @@
         <v>9</v>
       </c>
       <c r="B10" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C10" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D10" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="E10" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="F10" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="G10" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H10" s="2">
         <v>0</v>
@@ -1467,7 +1515,7 @@
         <v>0.1</v>
       </c>
       <c r="J10" s="3">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -1478,16 +1526,16 @@
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D11" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E11" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="F11" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="G11" s="2">
         <v>1</v>
@@ -1496,10 +1544,10 @@
         <v>0</v>
       </c>
       <c r="I11">
-        <v>0.13</v>
+        <v>0.1</v>
       </c>
       <c r="J11" s="3">
-        <v>0.13</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -1510,16 +1558,16 @@
         <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D12" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="E12" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="F12" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="G12" s="2">
         <v>1</v>
@@ -1528,10 +1576,10 @@
         <v>0</v>
       </c>
       <c r="I12">
-        <v>0.22</v>
+        <v>0.13</v>
       </c>
       <c r="J12" s="3">
-        <v>0.22</v>
+        <v>0.13</v>
       </c>
     </row>
     <row r="13" spans="1:10">
@@ -1542,16 +1590,16 @@
         <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D13" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="E13" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="F13" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="G13" s="2">
         <v>1</v>
@@ -1560,10 +1608,10 @@
         <v>0</v>
       </c>
       <c r="I13">
-        <v>0.19</v>
+        <v>0.22</v>
       </c>
       <c r="J13" s="3">
-        <v>0.19</v>
+        <v>0.22</v>
       </c>
     </row>
     <row r="14" spans="1:10">
@@ -1574,16 +1622,16 @@
         <v>1</v>
       </c>
       <c r="C14" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D14" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="E14" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="F14" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="G14" s="2">
         <v>1</v>
@@ -1592,10 +1640,10 @@
         <v>0</v>
       </c>
       <c r="I14">
-        <v>0.1</v>
+        <v>0.19</v>
       </c>
       <c r="J14" s="3">
-        <v>0.1</v>
+        <v>0.19</v>
       </c>
     </row>
     <row r="15" spans="1:10">
@@ -1606,16 +1654,16 @@
         <v>1</v>
       </c>
       <c r="C15" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D15" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="E15" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="F15" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="G15" s="2">
         <v>1</v>
@@ -1624,10 +1672,10 @@
         <v>0</v>
       </c>
       <c r="I15">
-        <v>0.46</v>
+        <v>0.1</v>
       </c>
       <c r="J15" s="3">
-        <v>0.46</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="16" spans="1:10">
@@ -1638,16 +1686,16 @@
         <v>1</v>
       </c>
       <c r="C16" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D16" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="E16" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="F16" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="G16" s="2">
         <v>1</v>
@@ -1656,10 +1704,10 @@
         <v>0</v>
       </c>
       <c r="I16">
-        <v>0.1</v>
+        <v>0.46</v>
       </c>
       <c r="J16" s="3">
-        <v>0.1</v>
+        <v>0.46</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -1667,31 +1715,31 @@
         <v>16</v>
       </c>
       <c r="B17" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C17" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="D17" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="E17" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="F17" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="G17" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H17" s="2">
         <v>0</v>
       </c>
       <c r="I17">
-        <v>0.28999999999999998</v>
+        <v>0.1</v>
       </c>
       <c r="J17" s="3">
-        <v>0.57999999999999996</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="18" spans="1:10">
@@ -1699,31 +1747,31 @@
         <v>17</v>
       </c>
       <c r="B18" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C18" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D18" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E18" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F18" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="G18" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H18" s="2">
         <v>0</v>
       </c>
       <c r="I18">
-        <v>0.27</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="J18" s="3">
-        <v>0.27</v>
+        <v>0.57999999999999996</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -1734,16 +1782,16 @@
         <v>1</v>
       </c>
       <c r="C19" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="D19" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="E19" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="F19" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="G19" s="2">
         <v>1</v>
@@ -1752,10 +1800,10 @@
         <v>0</v>
       </c>
       <c r="I19">
-        <v>0.48</v>
+        <v>0.27</v>
       </c>
       <c r="J19" s="3">
-        <v>0.48</v>
+        <v>0.27</v>
       </c>
     </row>
     <row r="20" spans="1:10">
@@ -1763,31 +1811,31 @@
         <v>19</v>
       </c>
       <c r="B20" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C20" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D20" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="E20" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="F20" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="G20" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H20" s="2">
         <v>0</v>
       </c>
       <c r="I20">
-        <v>0.35</v>
+        <v>0.48</v>
       </c>
       <c r="J20" s="3">
-        <v>0.7</v>
+        <v>0.48</v>
       </c>
     </row>
     <row r="21" spans="1:10">
@@ -1798,16 +1846,16 @@
         <v>1</v>
       </c>
       <c r="C21" t="s">
-        <v>86</v>
+        <v>257</v>
       </c>
       <c r="D21" t="s">
-        <v>87</v>
+        <v>258</v>
       </c>
       <c r="E21" t="s">
-        <v>88</v>
+        <v>259</v>
       </c>
       <c r="F21" t="s">
-        <v>89</v>
+        <v>260</v>
       </c>
       <c r="G21" s="2">
         <v>1</v>
@@ -1816,10 +1864,10 @@
         <v>0</v>
       </c>
       <c r="I21">
-        <v>0.45</v>
+        <v>0.34</v>
       </c>
       <c r="J21" s="3">
-        <v>0.45</v>
+        <v>0.34</v>
       </c>
     </row>
     <row r="22" spans="1:10">
@@ -1830,16 +1878,16 @@
         <v>1</v>
       </c>
       <c r="C22" t="s">
-        <v>90</v>
+        <v>253</v>
       </c>
       <c r="D22" t="s">
-        <v>91</v>
+        <v>254</v>
       </c>
       <c r="E22" t="s">
-        <v>92</v>
+        <v>255</v>
       </c>
       <c r="F22" t="s">
-        <v>93</v>
+        <v>256</v>
       </c>
       <c r="G22" s="2">
         <v>1</v>
@@ -1848,10 +1896,10 @@
         <v>0</v>
       </c>
       <c r="I22">
-        <v>2.2000000000000002</v>
+        <v>0.47</v>
       </c>
       <c r="J22" s="3">
-        <v>2.2000000000000002</v>
+        <v>0.47</v>
       </c>
     </row>
     <row r="23" spans="1:10">
@@ -1862,16 +1910,16 @@
         <v>2</v>
       </c>
       <c r="C23" t="s">
-        <v>94</v>
-      </c>
-      <c r="D23" s="5">
-        <v>1935161</v>
+        <v>82</v>
+      </c>
+      <c r="D23" t="s">
+        <v>83</v>
       </c>
       <c r="E23" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="F23" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="G23" s="2">
         <v>2</v>
@@ -1880,10 +1928,10 @@
         <v>0</v>
       </c>
       <c r="I23">
-        <v>0.43</v>
+        <v>0.35</v>
       </c>
       <c r="J23" s="3">
-        <v>0.86</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="24" spans="1:10">
@@ -1894,16 +1942,16 @@
         <v>1</v>
       </c>
       <c r="C24" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="D24" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="E24" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="F24" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="G24" s="2">
         <v>1</v>
@@ -1912,10 +1960,10 @@
         <v>0</v>
       </c>
       <c r="I24">
-        <v>0.42</v>
+        <v>0.45</v>
       </c>
       <c r="J24" s="3">
-        <v>0.42</v>
+        <v>0.45</v>
       </c>
     </row>
     <row r="25" spans="1:10">
@@ -1926,16 +1974,16 @@
         <v>1</v>
       </c>
       <c r="C25" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="D25" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="E25" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
       <c r="F25" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
       <c r="G25" s="2">
         <v>1</v>
@@ -1944,10 +1992,10 @@
         <v>0</v>
       </c>
       <c r="I25">
-        <v>0.24</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="J25" s="3">
-        <v>0.24</v>
+        <v>2.2000000000000002</v>
       </c>
     </row>
     <row r="26" spans="1:10">
@@ -1955,31 +2003,31 @@
         <v>25</v>
       </c>
       <c r="B26" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C26" t="s">
-        <v>105</v>
-      </c>
-      <c r="D26" t="s">
-        <v>106</v>
+        <v>94</v>
+      </c>
+      <c r="D26" s="5">
+        <v>1935161</v>
       </c>
       <c r="E26" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="F26" t="s">
-        <v>108</v>
+        <v>96</v>
       </c>
       <c r="G26" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H26" s="2">
         <v>0</v>
       </c>
       <c r="I26">
-        <v>0.1</v>
+        <v>0.43</v>
       </c>
       <c r="J26" s="3">
-        <v>0.1</v>
+        <v>0.86</v>
       </c>
     </row>
     <row r="27" spans="1:10">
@@ -1990,16 +2038,16 @@
         <v>1</v>
       </c>
       <c r="C27" t="s">
-        <v>109</v>
+        <v>97</v>
       </c>
       <c r="D27" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="E27" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="F27" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="G27" s="2">
         <v>1</v>
@@ -2008,10 +2056,10 @@
         <v>0</v>
       </c>
       <c r="I27">
-        <v>0.23</v>
+        <v>0.42</v>
       </c>
       <c r="J27" s="3">
-        <v>0.23</v>
+        <v>0.42</v>
       </c>
     </row>
     <row r="28" spans="1:10">
@@ -2022,16 +2070,16 @@
         <v>1</v>
       </c>
       <c r="C28" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
       <c r="D28" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="E28" t="s">
-        <v>115</v>
+        <v>103</v>
       </c>
       <c r="F28" t="s">
-        <v>116</v>
+        <v>104</v>
       </c>
       <c r="G28" s="2">
         <v>1</v>
@@ -2040,10 +2088,10 @@
         <v>0</v>
       </c>
       <c r="I28">
-        <v>0.16</v>
+        <v>0.24</v>
       </c>
       <c r="J28" s="3">
-        <v>0.16</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="29" spans="1:10">
@@ -2054,16 +2102,16 @@
         <v>1</v>
       </c>
       <c r="C29" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
       <c r="D29" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
       <c r="E29" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
       <c r="F29" t="s">
-        <v>120</v>
+        <v>108</v>
       </c>
       <c r="G29" s="2">
         <v>1</v>
@@ -2072,10 +2120,10 @@
         <v>0</v>
       </c>
       <c r="I29">
-        <v>0.89</v>
+        <v>0.1</v>
       </c>
       <c r="J29" s="3">
-        <v>0.89</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="30" spans="1:10">
@@ -2086,16 +2134,16 @@
         <v>1</v>
       </c>
       <c r="C30" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
       <c r="D30" t="s">
-        <v>122</v>
+        <v>110</v>
       </c>
       <c r="E30" t="s">
-        <v>123</v>
+        <v>111</v>
       </c>
       <c r="F30" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
       <c r="G30" s="2">
         <v>1</v>
@@ -2104,10 +2152,10 @@
         <v>0</v>
       </c>
       <c r="I30">
-        <v>0.28000000000000003</v>
+        <v>0.23</v>
       </c>
       <c r="J30" s="3">
-        <v>0.28000000000000003</v>
+        <v>0.23</v>
       </c>
     </row>
     <row r="31" spans="1:10">
@@ -2115,31 +2163,31 @@
         <v>30</v>
       </c>
       <c r="B31" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C31" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="D31" t="s">
-        <v>126</v>
+        <v>114</v>
       </c>
       <c r="E31" t="s">
-        <v>127</v>
+        <v>115</v>
       </c>
       <c r="F31" t="s">
-        <v>128</v>
+        <v>116</v>
       </c>
       <c r="G31" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H31" s="2">
         <v>0</v>
       </c>
       <c r="I31">
-        <v>0.59</v>
+        <v>0.16</v>
       </c>
       <c r="J31" s="3">
-        <v>2.36</v>
+        <v>0.16</v>
       </c>
     </row>
     <row r="32" spans="1:10">
@@ -2150,16 +2198,16 @@
         <v>1</v>
       </c>
       <c r="C32" t="s">
-        <v>129</v>
+        <v>117</v>
       </c>
       <c r="D32" t="s">
-        <v>130</v>
+        <v>118</v>
       </c>
       <c r="E32" t="s">
-        <v>131</v>
+        <v>119</v>
       </c>
       <c r="F32" t="s">
-        <v>132</v>
+        <v>120</v>
       </c>
       <c r="G32" s="2">
         <v>1</v>
@@ -2168,10 +2216,10 @@
         <v>0</v>
       </c>
       <c r="I32">
-        <v>0.51</v>
+        <v>0.89</v>
       </c>
       <c r="J32" s="3">
-        <v>0.51</v>
+        <v>0.89</v>
       </c>
     </row>
     <row r="33" spans="1:10">
@@ -2179,31 +2227,31 @@
         <v>32</v>
       </c>
       <c r="B33" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C33" t="s">
-        <v>133</v>
+        <v>121</v>
       </c>
       <c r="D33" t="s">
-        <v>134</v>
+        <v>122</v>
       </c>
       <c r="E33" t="s">
-        <v>135</v>
+        <v>123</v>
       </c>
       <c r="F33" t="s">
-        <v>136</v>
+        <v>124</v>
       </c>
       <c r="G33" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H33" s="2">
         <v>0</v>
       </c>
       <c r="I33">
-        <v>0.1</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="J33" s="3">
-        <v>0.3</v>
+        <v>0.28000000000000003</v>
       </c>
     </row>
     <row r="34" spans="1:10">
@@ -2211,31 +2259,31 @@
         <v>33</v>
       </c>
       <c r="B34" s="2">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C34" t="s">
-        <v>137</v>
+        <v>125</v>
       </c>
       <c r="D34" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
       <c r="E34" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
       <c r="F34" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
       <c r="G34" s="2">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H34" s="2">
         <v>0</v>
       </c>
       <c r="I34">
-        <v>0.1</v>
+        <v>0.59</v>
       </c>
       <c r="J34" s="3">
-        <v>0.1</v>
+        <v>2.36</v>
       </c>
     </row>
     <row r="35" spans="1:10">
@@ -2243,31 +2291,31 @@
         <v>34</v>
       </c>
       <c r="B35" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C35" t="s">
-        <v>141</v>
+        <v>129</v>
       </c>
       <c r="D35" t="s">
-        <v>142</v>
+        <v>130</v>
       </c>
       <c r="E35" t="s">
-        <v>143</v>
+        <v>131</v>
       </c>
       <c r="F35" t="s">
-        <v>144</v>
+        <v>132</v>
       </c>
       <c r="G35" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H35" s="2">
         <v>0</v>
       </c>
       <c r="I35">
-        <v>0.1</v>
+        <v>0.51</v>
       </c>
       <c r="J35" s="3">
-        <v>0.2</v>
+        <v>0.51</v>
       </c>
     </row>
     <row r="36" spans="1:10">
@@ -2275,22 +2323,22 @@
         <v>35</v>
       </c>
       <c r="B36" s="2">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C36" t="s">
-        <v>145</v>
+        <v>133</v>
       </c>
       <c r="D36" t="s">
-        <v>146</v>
+        <v>134</v>
       </c>
       <c r="E36" t="s">
-        <v>147</v>
+        <v>135</v>
       </c>
       <c r="F36" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="G36" s="2">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="H36" s="2">
         <v>0</v>
@@ -2299,7 +2347,7 @@
         <v>0.1</v>
       </c>
       <c r="J36" s="3">
-        <v>0.8</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="37" spans="1:10">
@@ -2307,31 +2355,31 @@
         <v>36</v>
       </c>
       <c r="B37" s="2">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="C37" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="D37" t="s">
-        <v>150</v>
+        <v>138</v>
       </c>
       <c r="E37" t="s">
-        <v>151</v>
+        <v>139</v>
       </c>
       <c r="F37" t="s">
-        <v>152</v>
+        <v>140</v>
       </c>
       <c r="G37" s="2">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="H37" s="2">
         <v>0</v>
       </c>
       <c r="I37">
-        <v>1.7000000000000001E-2</v>
+        <v>0.1</v>
       </c>
       <c r="J37" s="3">
-        <v>0.19</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="38" spans="1:10">
@@ -2339,22 +2387,22 @@
         <v>37</v>
       </c>
       <c r="B38" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C38" t="s">
-        <v>153</v>
+        <v>141</v>
       </c>
       <c r="D38" t="s">
-        <v>154</v>
+        <v>142</v>
       </c>
       <c r="E38" t="s">
-        <v>155</v>
+        <v>143</v>
       </c>
       <c r="F38" t="s">
-        <v>156</v>
+        <v>144</v>
       </c>
       <c r="G38" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H38" s="2">
         <v>0</v>
@@ -2363,7 +2411,7 @@
         <v>0.1</v>
       </c>
       <c r="J38" s="3">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="39" spans="1:10">
@@ -2371,22 +2419,22 @@
         <v>38</v>
       </c>
       <c r="B39" s="2">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C39" t="s">
-        <v>243</v>
+        <v>145</v>
       </c>
       <c r="D39" t="s">
-        <v>244</v>
+        <v>146</v>
       </c>
       <c r="E39" t="s">
-        <v>245</v>
+        <v>147</v>
       </c>
       <c r="F39" t="s">
-        <v>242</v>
+        <v>148</v>
       </c>
       <c r="G39" s="2">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="H39" s="2">
         <v>0</v>
@@ -2395,7 +2443,7 @@
         <v>0.1</v>
       </c>
       <c r="J39" s="3">
-        <v>0.1</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="40" spans="1:10">
@@ -2403,31 +2451,31 @@
         <v>39</v>
       </c>
       <c r="B40" s="2">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="C40" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="D40" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="E40" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="F40" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="G40" s="2">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="H40" s="2">
         <v>0</v>
       </c>
       <c r="I40">
-        <v>0.24</v>
+        <v>1.7000000000000001E-2</v>
       </c>
       <c r="J40" s="3">
-        <v>0.96</v>
+        <v>0.19</v>
       </c>
     </row>
     <row r="41" spans="1:10">
@@ -2438,16 +2486,16 @@
         <v>1</v>
       </c>
       <c r="C41" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="D41" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="E41" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="F41" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="G41" s="2">
         <v>1</v>
@@ -2470,16 +2518,16 @@
         <v>1</v>
       </c>
       <c r="C42" t="s">
-        <v>165</v>
+        <v>242</v>
       </c>
       <c r="D42" t="s">
-        <v>166</v>
+        <v>243</v>
       </c>
       <c r="E42" t="s">
-        <v>167</v>
+        <v>244</v>
       </c>
       <c r="F42" t="s">
-        <v>168</v>
+        <v>241</v>
       </c>
       <c r="G42" s="2">
         <v>1</v>
@@ -2499,31 +2547,31 @@
         <v>42</v>
       </c>
       <c r="B43" s="2">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C43" t="s">
-        <v>169</v>
+        <v>157</v>
       </c>
       <c r="D43" t="s">
-        <v>170</v>
+        <v>158</v>
       </c>
       <c r="E43" t="s">
-        <v>171</v>
+        <v>159</v>
       </c>
       <c r="F43" t="s">
-        <v>172</v>
+        <v>160</v>
       </c>
       <c r="G43" s="2">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H43" s="2">
         <v>0</v>
       </c>
       <c r="I43">
-        <v>0.1</v>
+        <v>0.24</v>
       </c>
       <c r="J43" s="3">
-        <v>0.1</v>
+        <v>0.96</v>
       </c>
     </row>
     <row r="44" spans="1:10">
@@ -2534,16 +2582,16 @@
         <v>1</v>
       </c>
       <c r="C44" t="s">
-        <v>173</v>
+        <v>161</v>
       </c>
       <c r="D44" t="s">
-        <v>174</v>
+        <v>162</v>
       </c>
       <c r="E44" t="s">
-        <v>175</v>
+        <v>163</v>
       </c>
       <c r="F44" t="s">
-        <v>176</v>
+        <v>164</v>
       </c>
       <c r="G44" s="2">
         <v>1</v>
@@ -2566,16 +2614,16 @@
         <v>1</v>
       </c>
       <c r="C45" t="s">
-        <v>177</v>
+        <v>165</v>
       </c>
       <c r="D45" t="s">
-        <v>178</v>
+        <v>166</v>
       </c>
       <c r="E45" t="s">
-        <v>179</v>
+        <v>167</v>
       </c>
       <c r="F45" t="s">
-        <v>180</v>
+        <v>168</v>
       </c>
       <c r="G45" s="2">
         <v>1</v>
@@ -2598,16 +2646,16 @@
         <v>1</v>
       </c>
       <c r="C46" t="s">
-        <v>181</v>
+        <v>169</v>
       </c>
       <c r="D46" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
       <c r="E46" t="s">
-        <v>183</v>
+        <v>171</v>
       </c>
       <c r="F46" t="s">
-        <v>184</v>
+        <v>172</v>
       </c>
       <c r="G46" s="2">
         <v>1</v>
@@ -2616,10 +2664,10 @@
         <v>0</v>
       </c>
       <c r="I46">
-        <v>0.52</v>
+        <v>0.1</v>
       </c>
       <c r="J46" s="3">
-        <v>0.52</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="47" spans="1:10">
@@ -2630,16 +2678,16 @@
         <v>1</v>
       </c>
       <c r="C47" t="s">
-        <v>185</v>
+        <v>173</v>
       </c>
       <c r="D47" t="s">
-        <v>186</v>
+        <v>174</v>
       </c>
       <c r="E47" t="s">
-        <v>187</v>
+        <v>175</v>
       </c>
       <c r="F47" t="s">
-        <v>188</v>
+        <v>176</v>
       </c>
       <c r="G47" s="2">
         <v>1</v>
@@ -2648,10 +2696,10 @@
         <v>0</v>
       </c>
       <c r="I47">
-        <v>0.11</v>
+        <v>0.1</v>
       </c>
       <c r="J47" s="3">
-        <v>0.11</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="48" spans="1:10">
@@ -2662,16 +2710,16 @@
         <v>1</v>
       </c>
       <c r="C48" t="s">
-        <v>189</v>
+        <v>249</v>
       </c>
       <c r="D48" t="s">
-        <v>190</v>
+        <v>250</v>
       </c>
       <c r="E48" t="s">
-        <v>191</v>
+        <v>251</v>
       </c>
       <c r="F48" t="s">
-        <v>192</v>
+        <v>252</v>
       </c>
       <c r="G48" s="2">
         <v>1</v>
@@ -2680,10 +2728,10 @@
         <v>0</v>
       </c>
       <c r="I48">
-        <v>1.99</v>
+        <v>0.1</v>
       </c>
       <c r="J48" s="3">
-        <v>1.99</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="49" spans="1:10">
@@ -2694,16 +2742,16 @@
         <v>1</v>
       </c>
       <c r="C49" t="s">
-        <v>193</v>
+        <v>177</v>
       </c>
       <c r="D49" t="s">
-        <v>194</v>
+        <v>178</v>
       </c>
       <c r="E49" t="s">
-        <v>195</v>
+        <v>179</v>
       </c>
       <c r="F49" t="s">
-        <v>196</v>
+        <v>180</v>
       </c>
       <c r="G49" s="2">
         <v>1</v>
@@ -2712,10 +2760,10 @@
         <v>0</v>
       </c>
       <c r="I49">
-        <v>2.04</v>
+        <v>0.1</v>
       </c>
       <c r="J49" s="3">
-        <v>2.04</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="50" spans="1:10">
@@ -2726,16 +2774,16 @@
         <v>1</v>
       </c>
       <c r="C50" t="s">
-        <v>197</v>
+        <v>181</v>
       </c>
       <c r="D50" t="s">
-        <v>198</v>
+        <v>182</v>
       </c>
       <c r="E50" t="s">
-        <v>199</v>
+        <v>183</v>
       </c>
       <c r="F50" t="s">
-        <v>200</v>
+        <v>184</v>
       </c>
       <c r="G50" s="2">
         <v>1</v>
@@ -2744,10 +2792,10 @@
         <v>0</v>
       </c>
       <c r="I50">
-        <v>2.96</v>
+        <v>0.52</v>
       </c>
       <c r="J50" s="3">
-        <v>2.96</v>
+        <v>0.52</v>
       </c>
     </row>
     <row r="51" spans="1:10">
@@ -2755,31 +2803,31 @@
         <v>50</v>
       </c>
       <c r="B51" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C51" t="s">
-        <v>201</v>
+        <v>185</v>
       </c>
       <c r="D51" t="s">
-        <v>202</v>
+        <v>186</v>
       </c>
       <c r="E51" t="s">
-        <v>203</v>
+        <v>187</v>
       </c>
       <c r="F51" t="s">
-        <v>204</v>
+        <v>188</v>
       </c>
       <c r="G51" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H51" s="2">
         <v>0</v>
       </c>
       <c r="I51">
-        <v>1.71</v>
+        <v>0.11</v>
       </c>
       <c r="J51" s="3">
-        <v>3.42</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="52" spans="1:10">
@@ -2790,16 +2838,16 @@
         <v>1</v>
       </c>
       <c r="C52" t="s">
-        <v>205</v>
+        <v>189</v>
       </c>
       <c r="D52" t="s">
-        <v>206</v>
+        <v>190</v>
       </c>
       <c r="E52" t="s">
-        <v>207</v>
+        <v>191</v>
       </c>
       <c r="F52" t="s">
-        <v>208</v>
+        <v>192</v>
       </c>
       <c r="G52" s="2">
         <v>1</v>
@@ -2808,10 +2856,10 @@
         <v>0</v>
       </c>
       <c r="I52">
-        <v>1.6</v>
+        <v>1.99</v>
       </c>
       <c r="J52" s="3">
-        <v>1.6</v>
+        <v>1.99</v>
       </c>
     </row>
     <row r="53" spans="1:10">
@@ -2819,31 +2867,31 @@
         <v>52</v>
       </c>
       <c r="B53" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C53" t="s">
-        <v>209</v>
+        <v>193</v>
       </c>
       <c r="D53" t="s">
-        <v>210</v>
+        <v>194</v>
       </c>
       <c r="E53" t="s">
-        <v>211</v>
+        <v>195</v>
       </c>
       <c r="F53" t="s">
-        <v>212</v>
+        <v>196</v>
       </c>
       <c r="G53" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H53" s="2">
         <v>0</v>
       </c>
       <c r="I53">
-        <v>2.9</v>
+        <v>2.04</v>
       </c>
       <c r="J53" s="3">
-        <v>8.6999999999999993</v>
+        <v>2.04</v>
       </c>
     </row>
     <row r="54" spans="1:10">
@@ -2854,16 +2902,16 @@
         <v>1</v>
       </c>
       <c r="C54" t="s">
-        <v>213</v>
+        <v>197</v>
       </c>
       <c r="D54" t="s">
-        <v>214</v>
+        <v>198</v>
       </c>
       <c r="E54" t="s">
-        <v>215</v>
+        <v>199</v>
       </c>
       <c r="F54" t="s">
-        <v>216</v>
+        <v>200</v>
       </c>
       <c r="G54" s="2">
         <v>1</v>
@@ -2872,10 +2920,10 @@
         <v>0</v>
       </c>
       <c r="I54">
-        <v>0.65</v>
+        <v>2.96</v>
       </c>
       <c r="J54" s="3">
-        <v>0.65</v>
+        <v>2.96</v>
       </c>
     </row>
     <row r="55" spans="1:10">
@@ -2883,31 +2931,31 @@
         <v>54</v>
       </c>
       <c r="B55" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C55" t="s">
-        <v>217</v>
+        <v>201</v>
       </c>
       <c r="D55" t="s">
-        <v>218</v>
+        <v>202</v>
       </c>
       <c r="E55" t="s">
-        <v>219</v>
+        <v>203</v>
       </c>
       <c r="F55" t="s">
-        <v>220</v>
+        <v>204</v>
       </c>
       <c r="G55" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H55" s="2">
         <v>0</v>
       </c>
       <c r="I55">
-        <v>5.54</v>
+        <v>1.71</v>
       </c>
       <c r="J55" s="3">
-        <v>5.54</v>
+        <v>3.42</v>
       </c>
     </row>
     <row r="56" spans="1:10">
@@ -2918,16 +2966,16 @@
         <v>1</v>
       </c>
       <c r="C56" t="s">
-        <v>221</v>
+        <v>205</v>
       </c>
       <c r="D56" t="s">
-        <v>222</v>
+        <v>206</v>
       </c>
       <c r="E56" t="s">
-        <v>223</v>
+        <v>207</v>
       </c>
       <c r="F56" t="s">
-        <v>224</v>
+        <v>208</v>
       </c>
       <c r="G56" s="2">
         <v>1</v>
@@ -2936,10 +2984,10 @@
         <v>0</v>
       </c>
       <c r="I56">
-        <v>7.12</v>
+        <v>1.6</v>
       </c>
       <c r="J56" s="3">
-        <v>7.12</v>
+        <v>1.6</v>
       </c>
     </row>
     <row r="57" spans="1:10">
@@ -2947,31 +2995,31 @@
         <v>56</v>
       </c>
       <c r="B57" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C57" t="s">
-        <v>225</v>
+        <v>209</v>
       </c>
       <c r="D57" t="s">
-        <v>226</v>
+        <v>210</v>
       </c>
       <c r="E57" t="s">
-        <v>227</v>
+        <v>211</v>
       </c>
       <c r="F57" t="s">
-        <v>228</v>
+        <v>261</v>
       </c>
       <c r="G57" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H57" s="2">
         <v>0</v>
       </c>
       <c r="I57">
-        <v>1.55</v>
+        <v>2.9</v>
       </c>
       <c r="J57" s="3">
-        <v>1.55</v>
+        <v>8.6999999999999993</v>
       </c>
     </row>
     <row r="58" spans="1:10">
@@ -2982,16 +3030,16 @@
         <v>1</v>
       </c>
       <c r="C58" t="s">
-        <v>229</v>
+        <v>212</v>
       </c>
       <c r="D58" t="s">
-        <v>230</v>
+        <v>213</v>
       </c>
       <c r="E58" t="s">
-        <v>231</v>
+        <v>214</v>
       </c>
       <c r="F58" t="s">
-        <v>232</v>
+        <v>215</v>
       </c>
       <c r="G58" s="2">
         <v>1</v>
@@ -3000,10 +3048,10 @@
         <v>0</v>
       </c>
       <c r="I58">
-        <v>0.28999999999999998</v>
+        <v>0.65</v>
       </c>
       <c r="J58" s="3">
-        <v>0.28999999999999998</v>
+        <v>0.65</v>
       </c>
     </row>
     <row r="59" spans="1:10">
@@ -3014,16 +3062,16 @@
         <v>1</v>
       </c>
       <c r="C59" t="s">
-        <v>233</v>
+        <v>216</v>
       </c>
       <c r="D59" t="s">
-        <v>234</v>
+        <v>217</v>
       </c>
       <c r="E59" t="s">
-        <v>235</v>
+        <v>218</v>
       </c>
       <c r="F59" t="s">
-        <v>236</v>
+        <v>219</v>
       </c>
       <c r="G59" s="2">
         <v>1</v>
@@ -3032,10 +3080,10 @@
         <v>0</v>
       </c>
       <c r="I59">
-        <v>7.18</v>
+        <v>5.54</v>
       </c>
       <c r="J59" s="3">
-        <v>7.18</v>
+        <v>5.54</v>
       </c>
     </row>
     <row r="60" spans="1:10">
@@ -3046,37 +3094,169 @@
         <v>1</v>
       </c>
       <c r="C60" t="s">
+        <v>220</v>
+      </c>
+      <c r="D60" t="s">
+        <v>221</v>
+      </c>
+      <c r="E60" t="s">
+        <v>222</v>
+      </c>
+      <c r="F60" t="s">
+        <v>223</v>
+      </c>
+      <c r="G60" s="2">
+        <v>1</v>
+      </c>
+      <c r="H60" s="2">
+        <v>0</v>
+      </c>
+      <c r="I60">
+        <v>7.12</v>
+      </c>
+      <c r="J60" s="3">
+        <v>7.12</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10">
+      <c r="A61" s="2">
+        <v>60</v>
+      </c>
+      <c r="B61" s="2">
+        <v>1</v>
+      </c>
+      <c r="C61" t="s">
+        <v>224</v>
+      </c>
+      <c r="D61" t="s">
+        <v>225</v>
+      </c>
+      <c r="E61" t="s">
+        <v>226</v>
+      </c>
+      <c r="F61" t="s">
+        <v>227</v>
+      </c>
+      <c r="G61" s="2">
+        <v>1</v>
+      </c>
+      <c r="H61" s="2">
+        <v>0</v>
+      </c>
+      <c r="I61">
+        <v>1.55</v>
+      </c>
+      <c r="J61" s="3">
+        <v>1.55</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10">
+      <c r="A62" s="2">
+        <v>61</v>
+      </c>
+      <c r="B62" s="2">
+        <v>1</v>
+      </c>
+      <c r="C62" t="s">
+        <v>228</v>
+      </c>
+      <c r="D62" t="s">
+        <v>229</v>
+      </c>
+      <c r="E62" t="s">
+        <v>230</v>
+      </c>
+      <c r="F62" t="s">
+        <v>231</v>
+      </c>
+      <c r="G62" s="2">
+        <v>1</v>
+      </c>
+      <c r="H62" s="2">
+        <v>0</v>
+      </c>
+      <c r="I62">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="J62" s="3">
+        <v>0.28999999999999998</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10">
+      <c r="A63" s="2">
+        <v>62</v>
+      </c>
+      <c r="B63" s="2">
+        <v>1</v>
+      </c>
+      <c r="C63" t="s">
+        <v>232</v>
+      </c>
+      <c r="D63" t="s">
+        <v>233</v>
+      </c>
+      <c r="E63" t="s">
+        <v>234</v>
+      </c>
+      <c r="F63" t="s">
+        <v>235</v>
+      </c>
+      <c r="G63" s="2">
+        <v>1</v>
+      </c>
+      <c r="H63" s="2">
+        <v>0</v>
+      </c>
+      <c r="I63">
+        <v>7.18</v>
+      </c>
+      <c r="J63" s="3">
+        <v>7.18</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10">
+      <c r="A64" s="2">
+        <v>63</v>
+      </c>
+      <c r="B64" s="2">
+        <v>1</v>
+      </c>
+      <c r="C64" t="s">
+        <v>236</v>
+      </c>
+      <c r="D64" t="s">
         <v>237</v>
       </c>
-      <c r="D60" t="s">
+      <c r="E64" t="s">
         <v>238</v>
       </c>
-      <c r="E60" t="s">
+      <c r="F64" t="s">
         <v>239</v>
       </c>
-      <c r="F60" t="s">
+      <c r="G64" s="2">
+        <v>1</v>
+      </c>
+      <c r="H64" s="2">
+        <v>0</v>
+      </c>
+      <c r="I64">
+        <v>0.44</v>
+      </c>
+      <c r="J64" s="3">
+        <v>0.44</v>
+      </c>
+    </row>
+    <row r="65" spans="7:10">
+      <c r="G65" s="2">
+        <f>SUM(G2:G64)</f>
+        <v>129</v>
+      </c>
+      <c r="I65" t="s">
         <v>240</v>
       </c>
-      <c r="G60" s="2">
-        <v>1</v>
-      </c>
-      <c r="H60" s="2">
-        <v>0</v>
-      </c>
-      <c r="I60">
-        <v>0.44</v>
-      </c>
-      <c r="J60" s="3">
-        <v>0.44</v>
-      </c>
-    </row>
-    <row r="61" spans="1:10">
-      <c r="I61" t="s">
-        <v>241</v>
-      </c>
-      <c r="J61" s="4">
-        <f>SUM(J2:J60)</f>
-        <v>62.18</v>
+      <c r="J65" s="4">
+        <f>SUM(J2:J64)</f>
+        <v>63.199999999999996</v>
       </c>
     </row>
   </sheetData>

</xml_diff>